<commit_message>
delete redundant records, update time in Logs.writeLog
</commit_message>
<xml_diff>
--- a/src/main/java/Log/channels.xlsx
+++ b/src/main/java/Log/channels.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -44,22 +44,103 @@
     <t>Users</t>
   </si>
   <si>
+    <t>"C05BWUFE1SN"</t>
+  </si>
+  <si>
+    <t>"ninh_test_channel"</t>
+  </si>
+  <si>
+    <t>"U059LLDK7LL"</t>
+  </si>
+  <si>
+    <t>"2023-06-10T05:09:46.000Z"</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>["recnpg0JcAfYQG2iv","recnHFluV9telxooz"]</t>
+  </si>
+  <si>
+    <t>"C05AWPHQ06T"</t>
+  </si>
+  <si>
+    <t>"test"</t>
+  </si>
+  <si>
+    <t>"2023-06-07T05:40:53.000Z"</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>["recnHFluV9telxooz"]</t>
+  </si>
+  <si>
+    <t>"C05BL6MJZJA"</t>
+  </si>
+  <si>
+    <t>"longggg23"</t>
+  </si>
+  <si>
+    <t>"2023-06-09T11:20:11.000Z"</t>
+  </si>
+  <si>
+    <t>"C057RLDG1L4"</t>
+  </si>
+  <si>
+    <t>"test-channel"</t>
+  </si>
+  <si>
+    <t>"U058B02DEJU"</t>
+  </si>
+  <si>
+    <t>"2023-05-14T10:51:18.000Z"</t>
+  </si>
+  <si>
+    <t>["recnpg0JcAfYQG2iv"]</t>
+  </si>
+  <si>
+    <t>"C05BBANJ96W"</t>
+  </si>
+  <si>
+    <t>"test1"</t>
+  </si>
+  <si>
+    <t>"2023-06-07T05:49:01.000Z"</t>
+  </si>
+  <si>
+    <t>"C05B4LN70KG"</t>
+  </si>
+  <si>
+    <t>"tes11t"</t>
+  </si>
+  <si>
+    <t>"2023-06-07T05:47:59.000Z"</t>
+  </si>
+  <si>
     <t>"C05C11EKV2L"</t>
   </si>
   <si>
     <t>"tes1t"</t>
   </si>
   <si>
-    <t>"U059LLDK7LL"</t>
-  </si>
-  <si>
     <t>"2023-06-07T05:43:20.000Z"</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>["recrfFnpsHp9TPFtk","recGF6jPu9TVSHD6c"]</t>
+    <t>"C057PPFRL6Q"</t>
+  </si>
+  <si>
+    <t>"general"</t>
+  </si>
+  <si>
+    <t>"2023-05-13T04:47:15.000Z"</t>
+  </si>
+  <si>
+    <t>"This is the one channel that will always include everyone. It?s a great spot for announcements and team-wide conversations."</t>
+  </si>
+  <si>
+    <t>["recnpg0JcAfYQG2iv","reczC5O2Fc7DW99Ou"]</t>
   </si>
   <si>
     <t>"C057ZTSR56V"</t>
@@ -68,79 +149,10 @@
     <t>"project1"</t>
   </si>
   <si>
-    <t>"U058B02DEJU"</t>
-  </si>
-  <si>
     <t>"2023-05-13T04:47:59.000Z"</t>
   </si>
   <si>
     <t>"This channel is for everything #project1. Hold meetings, share docs, and make decisions together with your team."</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>["recrfFnpsHp9TPFtk"]</t>
-  </si>
-  <si>
-    <t>"C057PPFRL6Q"</t>
-  </si>
-  <si>
-    <t>"general"</t>
-  </si>
-  <si>
-    <t>"2023-05-13T04:47:15.000Z"</t>
-  </si>
-  <si>
-    <t>"This is the one channel that will always include everyone. It?s a great spot for announcements and team-wide conversations."</t>
-  </si>
-  <si>
-    <t>"C05AWPHQ06T"</t>
-  </si>
-  <si>
-    <t>"test"</t>
-  </si>
-  <si>
-    <t>"2023-06-07T05:40:53.000Z"</t>
-  </si>
-  <si>
-    <t>["recGF6jPu9TVSHD6c"]</t>
-  </si>
-  <si>
-    <t>"C05BBANJ96W"</t>
-  </si>
-  <si>
-    <t>"test1"</t>
-  </si>
-  <si>
-    <t>"2023-06-07T05:49:01.000Z"</t>
-  </si>
-  <si>
-    <t>"C057RLDG1L4"</t>
-  </si>
-  <si>
-    <t>"test-channel"</t>
-  </si>
-  <si>
-    <t>"2023-05-14T10:51:18.000Z"</t>
-  </si>
-  <si>
-    <t>"C05BL6MJZJA"</t>
-  </si>
-  <si>
-    <t>"longggg23"</t>
-  </si>
-  <si>
-    <t>"2023-06-09T11:20:11.000Z"</t>
-  </si>
-  <si>
-    <t>"C05B4LN70KG"</t>
-  </si>
-  <si>
-    <t>"tes11t"</t>
-  </si>
-  <si>
-    <t>"2023-06-07T05:47:59.000Z"</t>
   </si>
   <si>
     <t>"C0576NKMLBH"</t>
@@ -194,7 +206,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -264,168 +276,166 @@
         <v>17</v>
       </c>
       <c r="C3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="D3" t="s" s="0">
-        <v>19</v>
-      </c>
       <c r="E3" s="0"/>
-      <c r="F3" t="s" s="0">
-        <v>20</v>
-      </c>
+      <c r="F3" s="0"/>
       <c r="G3" t="s" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
       <c r="J3" t="s" s="0">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>25</v>
-      </c>
       <c r="E4" s="0"/>
-      <c r="F4" t="s" s="0">
-        <v>26</v>
-      </c>
+      <c r="F4" s="0"/>
       <c r="G4" t="s" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H4" s="0"/>
       <c r="I4" s="0"/>
       <c r="J4" t="s" s="0">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>27</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>29</v>
       </c>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
       <c r="G5" t="s" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" s="0"/>
       <c r="I5" s="0"/>
       <c r="J5" t="s" s="0">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s" s="0">
         <v>31</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>33</v>
       </c>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="G6" t="s" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H6" s="0"/>
       <c r="I6" s="0"/>
       <c r="J6" t="s" s="0">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s" s="0">
         <v>34</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>36</v>
       </c>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="G7" t="s" s="0">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
       <c r="J7" t="s" s="0">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s" s="0">
         <v>37</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>39</v>
       </c>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="G8" t="s" s="0">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H8" s="0"/>
       <c r="I8" s="0"/>
       <c r="J8" t="s" s="0">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="E9" s="0"/>
+      <c r="F9" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="C9" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
       <c r="G9" t="s" s="0">
         <v>14</v>
       </c>
       <c r="H9" s="0"/>
       <c r="I9" s="0"/>
       <c r="J9" t="s" s="0">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
@@ -436,22 +446,48 @@
         <v>44</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E10" s="0"/>
       <c r="F10" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
       <c r="J10" t="s" s="0">
-        <v>22</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E11" s="0"/>
+      <c r="F11" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
+      <c r="J11" t="s" s="0">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>